<commit_message>
mais treinamentos de uma camada só
</commit_message>
<xml_diff>
--- a/Peaks-dataset-article/redes-ensemble-s/Teste04/better_results.xlsx
+++ b/Peaks-dataset-article/redes-ensemble-s/Teste04/better_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,1009 +527,1828 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>model_22_9_7</t>
+          <t>model_18_9_6</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9997735427952396</v>
+        <v>0.9971221851802489</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8534547500861769</v>
+        <v>0.8101195666964252</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9993299854719881</v>
+        <v>0.9888385405479932</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9992796260654657</v>
+        <v>0.9732373019069294</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9995126019313403</v>
+        <v>0.9890849748189917</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0003214231293374287</v>
+        <v>0.01924396095079473</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2079997095551038</v>
+        <v>1.269731331820006</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0005950044635148943</v>
+        <v>0.01999467953251867</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0007110608698974434</v>
+        <v>0.03998823093740465</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0006530315747155433</v>
+        <v>0.02999149551469408</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0546178350608918</v>
+        <v>0.5439643407311988</v>
       </c>
       <c r="N2" t="n">
-        <v>0.01792827736670282</v>
+        <v>0.1387226043253035</v>
       </c>
       <c r="O2" t="n">
-        <v>1.000013971652736</v>
+        <v>1.002092956232546</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01869152125085377</v>
+        <v>0.1446283127868105</v>
       </c>
       <c r="Q2" t="n">
-        <v>842.0855042858293</v>
+        <v>121.9011159686192</v>
       </c>
       <c r="R2" t="n">
-        <v>1345.481219956396</v>
+        <v>191.3770379861066</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>model_22_9_8</t>
+          <t>model_18_9_5</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9997733662200464</v>
+        <v>0.9971181670282211</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8536790466810209</v>
+        <v>0.8099476839269765</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9992225433726208</v>
+        <v>0.9902412618509765</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9992393103296912</v>
+        <v>0.9758073857824764</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9994621438299516</v>
+        <v>0.9902409762963744</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0003216737521921262</v>
+        <v>0.01927083035190641</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2076813530979058</v>
+        <v>1.270880712690757</v>
       </c>
       <c r="J3" t="n">
-        <v>0.000690418109070703</v>
+        <v>0.01748183942884006</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0007508553998993933</v>
+        <v>0.03614806851482425</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0007206369583348119</v>
+        <v>0.02681512051335846</v>
       </c>
       <c r="M3" t="n">
-        <v>0.05085987027780254</v>
+        <v>0.5272381417584484</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01793526560138227</v>
+        <v>0.1388194163361394</v>
       </c>
       <c r="O3" t="n">
-        <v>1.000013982546835</v>
+        <v>1.00209587852493</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01869880698915117</v>
+        <v>0.1447292462853761</v>
       </c>
       <c r="Q3" t="n">
-        <v>842.0839454359914</v>
+        <v>121.898325414179</v>
       </c>
       <c r="R3" t="n">
-        <v>1345.479661106558</v>
+        <v>191.3742474316664</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>model_22_9_9</t>
+          <t>model_18_9_7</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9997708857164302</v>
+        <v>0.9971026322201757</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8538785985469226</v>
+        <v>0.8102586084901616</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9991187574968349</v>
+        <v>0.9873526533715959</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9992007414643671</v>
+        <v>0.9705333533293303</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9994135410683828</v>
+        <v>0.9878654709343029</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0003251944670022894</v>
+        <v>0.01937471168483721</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2073981181914648</v>
+        <v>1.268801558705062</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0007825848558511373</v>
+        <v>0.02265650328785222</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0007889256431626703</v>
+        <v>0.04402841103389088</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0007857564981189119</v>
+        <v>0.03334235771439246</v>
       </c>
       <c r="M4" t="n">
-        <v>0.04747471697922476</v>
+        <v>0.5602435461960468</v>
       </c>
       <c r="N4" t="n">
-        <v>0.01803314911495742</v>
+        <v>0.1391930734082598</v>
       </c>
       <c r="O4" t="n">
-        <v>1.000014135585619</v>
+        <v>1.002107176567145</v>
       </c>
       <c r="P4" t="n">
-        <v>0.01880085760654601</v>
+        <v>0.1451188107126335</v>
       </c>
       <c r="Q4" t="n">
-        <v>842.0621743891469</v>
+        <v>121.8875731692721</v>
       </c>
       <c r="R4" t="n">
-        <v>1345.457890059714</v>
+        <v>191.3634951867595</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>model_22_9_6</t>
+          <t>model_18_9_4</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9997705556121292</v>
+        <v>0.9970869939439687</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8532022215858097</v>
+        <v>0.8097388660966869</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9994397150571014</v>
+        <v>0.9915415711458146</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9993212768565715</v>
+        <v>0.978212431050002</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9995643093028377</v>
+        <v>0.9913188268719327</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0003256630021391189</v>
+        <v>0.01947928490984044</v>
       </c>
       <c r="I5" t="n">
-        <v>0.208358137104012</v>
+        <v>1.272277078483421</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0004975594228592668</v>
+        <v>0.01515246057339195</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0006699485442902188</v>
+        <v>0.03255450312622728</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0005837523789112587</v>
+        <v>0.02385348275565406</v>
       </c>
       <c r="M5" t="n">
-        <v>0.05879080007762785</v>
+        <v>0.510076807478779</v>
       </c>
       <c r="N5" t="n">
-        <v>0.01804613537960743</v>
+        <v>0.1395682088078816</v>
       </c>
       <c r="O5" t="n">
-        <v>1.000014155951951</v>
+        <v>1.002118549858932</v>
       </c>
       <c r="P5" t="n">
-        <v>0.01881439672336745</v>
+        <v>0.1455099164028544</v>
       </c>
       <c r="Q5" t="n">
-        <v>842.0592948940809</v>
+        <v>121.8768073807639</v>
       </c>
       <c r="R5" t="n">
-        <v>1345.455010564648</v>
+        <v>191.3527293982513</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>model_22_9_10</t>
+          <t>model_18_9_8</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9997667641359308</v>
+        <v>0.9970627564069963</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8540562363254669</v>
+        <v>0.8103686177625691</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9990195780354975</v>
+        <v>0.9858003889413109</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9991641612583444</v>
+        <v>0.9677247517642037</v>
       </c>
       <c r="G6" t="n">
-        <v>0.999367198149245</v>
+        <v>0.9865957812597399</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0003310444522272507</v>
+        <v>0.01964136143117945</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2071459871509503</v>
+        <v>1.268065926193927</v>
       </c>
       <c r="J6" t="n">
-        <v>0.000870660889605</v>
+        <v>0.02543723550004473</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0008250329367065158</v>
+        <v>0.04822496130721778</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0008478482284877287</v>
+        <v>0.03683111670012213</v>
       </c>
       <c r="M6" t="n">
-        <v>0.04443492416787045</v>
+        <v>0.576044783609774</v>
       </c>
       <c r="N6" t="n">
-        <v>0.01819462701533754</v>
+        <v>0.1401476415469752</v>
       </c>
       <c r="O6" t="n">
-        <v>1.000014389873362</v>
+        <v>1.002136177158548</v>
       </c>
       <c r="P6" t="n">
-        <v>0.01896920995545065</v>
+        <v>0.1461140167932424</v>
       </c>
       <c r="Q6" t="n">
-        <v>842.0265157896903</v>
+        <v>121.8602353183036</v>
       </c>
       <c r="R6" t="n">
-        <v>1345.422231460257</v>
+        <v>191.336157335791</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>model_22_9_5</t>
+          <t>model_18_9_3</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9997633163694918</v>
+        <v>0.997024705866685</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8529176445093882</v>
+        <v>0.8094885386593688</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9995497563938098</v>
+        <v>0.9927188164049192</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9993636885294639</v>
+        <v>0.9804185008699939</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9996163986850612</v>
+        <v>0.9923023816977352</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0003359380562052841</v>
+        <v>0.01989580556944746</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2087620529544168</v>
+        <v>1.27395101920942</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0003998375321012418</v>
+        <v>0.01304353908438898</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0006280851736503217</v>
+        <v>0.02925824244581727</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0005139613528757817</v>
+        <v>0.02115094385562155</v>
       </c>
       <c r="M7" t="n">
-        <v>0.06343471411977647</v>
+        <v>0.4925233785772338</v>
       </c>
       <c r="N7" t="n">
-        <v>0.01832861304641691</v>
+        <v>0.1410524922482671</v>
       </c>
       <c r="O7" t="n">
-        <v>1.000014602589029</v>
+        <v>1.002163850278775</v>
       </c>
       <c r="P7" t="n">
-        <v>0.01910890004926239</v>
+        <v>0.1470573888621875</v>
       </c>
       <c r="Q7" t="n">
-        <v>841.9971675430575</v>
+        <v>121.8344926897452</v>
       </c>
       <c r="R7" t="n">
-        <v>1345.392883213624</v>
+        <v>191.3104147072326</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>model_22_9_4</t>
+          <t>model_18_9_2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9997504365126391</v>
+        <v>0.9969269485316756</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8525964631431158</v>
+        <v>0.8091917315306681</v>
       </c>
       <c r="E8" t="n">
-        <v>0.999657503429227</v>
+        <v>0.9937497509687674</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9994060159908327</v>
+        <v>0.982387225827796</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9996676979398783</v>
+        <v>0.9931737322650681</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0003542191433509788</v>
+        <v>0.02054950931878619</v>
       </c>
       <c r="I8" t="n">
-        <v>0.209217923280739</v>
+        <v>1.275935769845712</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0003041530889683757</v>
+        <v>0.01119671911323946</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0005863049258393546</v>
+        <v>0.02631661720343531</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0004452289648976248</v>
+        <v>0.01875671148340851</v>
       </c>
       <c r="M8" t="n">
-        <v>0.06859671046370525</v>
+        <v>0.4746089687689177</v>
       </c>
       <c r="N8" t="n">
-        <v>0.01882071049006862</v>
+        <v>0.1433510004108314</v>
       </c>
       <c r="O8" t="n">
-        <v>1.000015397233153</v>
+        <v>1.002234946522418</v>
       </c>
       <c r="P8" t="n">
-        <v>0.01962194709987249</v>
+        <v>0.1494537492758</v>
       </c>
       <c r="Q8" t="n">
-        <v>841.8911895746965</v>
+        <v>121.7698364315126</v>
       </c>
       <c r="R8" t="n">
-        <v>1345.286905245263</v>
+        <v>191.245758449</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>model_22_9_3</t>
+          <t>model_18_9_1</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9997301696369398</v>
+        <v>0.9967889512687224</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8522334759911255</v>
+        <v>0.8088430103661259</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9997594748528723</v>
+        <v>0.9946092762986221</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9994470809151198</v>
+        <v>0.9840774001768813</v>
       </c>
       <c r="G9" t="n">
-        <v>0.999716618812855</v>
+        <v>0.9939135008311663</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0003829850314402303</v>
+        <v>0.02147229765157319</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2097331308513057</v>
+        <v>1.278267669878719</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0002135976611630328</v>
+        <v>0.009656962274590866</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00054577089290721</v>
+        <v>0.02379119611320523</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0003796832092399649</v>
+        <v>0.01672403036136685</v>
       </c>
       <c r="M9" t="n">
-        <v>0.07485130550430483</v>
+        <v>0.4563942477296511</v>
       </c>
       <c r="N9" t="n">
-        <v>0.01957000335820692</v>
+        <v>0.1465342883135998</v>
       </c>
       <c r="O9" t="n">
-        <v>1.000016647631654</v>
+        <v>1.002335308168202</v>
       </c>
       <c r="P9" t="n">
-        <v>0.02040313891665751</v>
+        <v>0.1527725563349036</v>
       </c>
       <c r="Q9" t="n">
-        <v>841.7350293038977</v>
+        <v>121.681983311953</v>
       </c>
       <c r="R9" t="n">
-        <v>1345.130744974465</v>
+        <v>191.1579053294404</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>model_22_9_2</t>
+          <t>model_18_9_0</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9997003133011322</v>
+        <v>0.9966054173589985</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8518225699403054</v>
+        <v>0.8084364479870274</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9998510721748858</v>
+        <v>0.9952695461849034</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9994853815840958</v>
+        <v>0.9854444637712864</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9997610821655097</v>
+        <v>0.9945004179285987</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0004253617661349764</v>
+        <v>0.02269958975099234</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2103163523427924</v>
+        <v>1.280986354379798</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0001322549243036063</v>
+        <v>0.008474152370748608</v>
       </c>
       <c r="K10" t="n">
-        <v>0.000507965378723279</v>
+        <v>0.02174855995861883</v>
       </c>
       <c r="L10" t="n">
-        <v>0.000320109782367069</v>
+        <v>0.01511134315238366</v>
       </c>
       <c r="M10" t="n">
-        <v>0.08281026590129487</v>
+        <v>0.4379334140795146</v>
       </c>
       <c r="N10" t="n">
-        <v>0.02062430037928503</v>
+        <v>0.1506638302678926</v>
       </c>
       <c r="O10" t="n">
-        <v>1.000018489667796</v>
+        <v>1.002468787375274</v>
       </c>
       <c r="P10" t="n">
-        <v>0.02150231954461861</v>
+        <v>0.1570779014395209</v>
       </c>
       <c r="Q10" t="n">
-        <v>841.5251410733644</v>
+        <v>121.5708168546032</v>
       </c>
       <c r="R10" t="n">
-        <v>1344.920856743931</v>
+        <v>191.0467388720906</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>model_22_9_1</t>
+          <t>model_18_8_5</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9996581146346163</v>
+        <v>0.9965004703566351</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8513566288921136</v>
+        <v>0.8066080044818638</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9999264110144183</v>
+        <v>0.9713215422038393</v>
       </c>
       <c r="F11" t="n">
-        <v>0.999518804212096</v>
+        <v>0.9978714612608257</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9997983609110106</v>
+        <v>0.9961492428111429</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0004852566476413526</v>
+        <v>0.02340137083903328</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2109776880240968</v>
+        <v>1.293213164518036</v>
       </c>
       <c r="J11" t="n">
-        <v>6.53504857821053e-05</v>
+        <v>0.02910366328882528</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0004749748417246839</v>
+        <v>0.03051776738588199</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0002701625227384563</v>
+        <v>0.02981084995589258</v>
       </c>
       <c r="M11" t="n">
-        <v>0.09164219752813101</v>
+        <v>0.4148695822732287</v>
       </c>
       <c r="N11" t="n">
-        <v>0.02202854165943249</v>
+        <v>0.1529750660697137</v>
       </c>
       <c r="O11" t="n">
-        <v>1.000021093184497</v>
+        <v>1.002545112467902</v>
       </c>
       <c r="P11" t="n">
-        <v>0.02296634228324213</v>
+        <v>0.1594875313343433</v>
       </c>
       <c r="Q11" t="n">
-        <v>841.2616652731871</v>
+        <v>121.5099213509394</v>
       </c>
       <c r="R11" t="n">
-        <v>1344.657380943754</v>
+        <v>190.9858433684269</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>model_22_8_8</t>
+          <t>model_18_8_4</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9995843894839793</v>
+        <v>0.9963951526138238</v>
       </c>
       <c r="D12" t="n">
-        <v>0.852032394616165</v>
+        <v>0.8064214057057328</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9994335559774675</v>
+        <v>0.973987947461045</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9991486303415698</v>
+        <v>0.9980292765263654</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9994128404597629</v>
+        <v>0.9964701567877177</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0005898987969325631</v>
+        <v>0.02410563107015587</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2100185366738304</v>
+        <v>1.294460951393231</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0004792917946444691</v>
+        <v>0.02639772417073023</v>
       </c>
       <c r="K12" t="n">
-        <v>0.001412803526094982</v>
+        <v>0.02825510264079435</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0009460461875388231</v>
+        <v>0.02732647664040425</v>
       </c>
       <c r="M12" t="n">
-        <v>0.100915650340609</v>
+        <v>0.4198904124921566</v>
       </c>
       <c r="N12" t="n">
-        <v>0.02428783228146479</v>
+        <v>0.1552598823590816</v>
       </c>
       <c r="O12" t="n">
-        <v>1.000025641779909</v>
+        <v>1.002621707189946</v>
       </c>
       <c r="P12" t="n">
-        <v>0.02532181558443068</v>
+        <v>0.1618696169833713</v>
       </c>
       <c r="Q12" t="n">
-        <v>840.8711191328007</v>
+        <v>121.4506196228303</v>
       </c>
       <c r="R12" t="n">
-        <v>1344.266834803368</v>
+        <v>190.9265416403177</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>model_22_8_7</t>
+          <t>model_18_8_3</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9995640682612773</v>
+        <v>0.9962494947822356</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8522491716422277</v>
+        <v>0.8061854083605905</v>
       </c>
       <c r="E13" t="n">
-        <v>0.999515061217402</v>
+        <v>0.976526407944486</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9992519596158036</v>
+        <v>0.9981493141095867</v>
       </c>
       <c r="G13" t="n">
-        <v>0.9994874520825924</v>
+        <v>0.9967477074511442</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0006187418227031528</v>
+        <v>0.02507964566067909</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2097108531529671</v>
+        <v>1.296039066726867</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0004103268287040503</v>
+        <v>0.02382162681894218</v>
       </c>
       <c r="K13" t="n">
-        <v>0.001241333986934359</v>
+        <v>0.02653407263326294</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0008258300682616479</v>
+        <v>0.02517780281425185</v>
       </c>
       <c r="M13" t="n">
-        <v>0.09925943385141503</v>
+        <v>0.4252892822118293</v>
       </c>
       <c r="N13" t="n">
-        <v>0.02487452155727126</v>
+        <v>0.1583655444239027</v>
       </c>
       <c r="O13" t="n">
-        <v>1.000026895531438</v>
+        <v>1.002727640158374</v>
       </c>
       <c r="P13" t="n">
-        <v>0.02593348143732246</v>
+        <v>0.1651074935118985</v>
       </c>
       <c r="Q13" t="n">
-        <v>840.775644920004</v>
+        <v>121.3713973833586</v>
       </c>
       <c r="R13" t="n">
-        <v>1344.171360590571</v>
+        <v>190.847319400846</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>model_22_8_6</t>
+          <t>model_10_9_3</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.999533413254032</v>
+        <v>0.9960762697386704</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8524816996959228</v>
+        <v>0.8063203366369693</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9995971553440928</v>
+        <v>0.9972236965650358</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9993591605030978</v>
+        <v>0.97204193578899</v>
       </c>
       <c r="G14" t="n">
-        <v>0.999564213459769</v>
+        <v>0.9899572138409216</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0006622521555674636</v>
+        <v>0.02623800232462765</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2093808133348193</v>
+        <v>1.295136800721434</v>
       </c>
       <c r="J14" t="n">
-        <v>0.000340863581240508</v>
+        <v>0.01234090842827995</v>
       </c>
       <c r="K14" t="n">
-        <v>0.001063439707909864</v>
+        <v>0.05064386796096039</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0007021502108265363</v>
+        <v>0.03149253678027948</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0973947800824512</v>
+        <v>0.3337036350839358</v>
       </c>
       <c r="N14" t="n">
-        <v>0.02573426034622841</v>
+        <v>0.1619814875985143</v>
       </c>
       <c r="O14" t="n">
-        <v>1.000028786842939</v>
+        <v>1.003766781050876</v>
       </c>
       <c r="P14" t="n">
-        <v>0.02682982108643015</v>
+        <v>0.1688773748734877</v>
       </c>
       <c r="Q14" t="n">
-        <v>840.6397283498047</v>
+        <v>105.2810928974511</v>
       </c>
       <c r="R14" t="n">
-        <v>1344.035444020372</v>
+        <v>165.0060083159929</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[12], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>119</v>
+        <v>37</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>model_22_8_5</t>
+          <t>model_10_9_2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9994894063003672</v>
+        <v>0.9960622508315162</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8527297387658093</v>
+        <v>0.8058553087415219</v>
       </c>
       <c r="E15" t="n">
-        <v>0.999678294447975</v>
+        <v>0.9977497057656739</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9994688150064071</v>
+        <v>0.9764530481074827</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9996419858675643</v>
+        <v>0.9916041222902267</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0007247136381885009</v>
+        <v>0.02633174682131906</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2090287578807869</v>
+        <v>1.298246444399547</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0002722084182084318</v>
+        <v>0.01000275212455786</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0008814737811311441</v>
+        <v>0.04265347963748208</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0005768413554841829</v>
+        <v>0.02632810092632993</v>
       </c>
       <c r="M15" t="n">
-        <v>0.09529133640856662</v>
+        <v>0.3421348505412943</v>
       </c>
       <c r="N15" t="n">
-        <v>0.02692050590513672</v>
+        <v>0.1622705975256117</v>
       </c>
       <c r="O15" t="n">
-        <v>1.000031501924913</v>
+        <v>1.003780239201745</v>
       </c>
       <c r="P15" t="n">
-        <v>0.02806656757464802</v>
+        <v>0.1691787928087216</v>
       </c>
       <c r="Q15" t="n">
-        <v>840.4594679258888</v>
+        <v>105.2739599285797</v>
       </c>
       <c r="R15" t="n">
-        <v>1343.855183596456</v>
+        <v>164.9988753471215</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[12], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>120</v>
+        <v>38</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>model_22_8_4</t>
+          <t>model_18_8_2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.9994282501016635</v>
+        <v>0.9960575828526035</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8529926710287036</v>
+        <v>0.8058929429681044</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9997563853610871</v>
+        <v>0.978887311375406</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9995788232000742</v>
+        <v>0.9982254871711828</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9997191404767727</v>
+        <v>0.9969729881475476</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0008115159847357041</v>
+        <v>0.02636296161780264</v>
       </c>
       <c r="I16" t="n">
-        <v>0.208655563701195</v>
+        <v>1.2979947841531</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0002061324558853572</v>
+        <v>0.0214257190961731</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0006989209236581259</v>
+        <v>0.02544194697349797</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0004525279127302175</v>
+        <v>0.02343377983147985</v>
       </c>
       <c r="M16" t="n">
-        <v>0.09291977454238948</v>
+        <v>0.4337577057537411</v>
       </c>
       <c r="N16" t="n">
-        <v>0.02848711962862697</v>
+        <v>0.1623667503456377</v>
       </c>
       <c r="O16" t="n">
-        <v>1.000035275057995</v>
+        <v>1.002867212470834</v>
       </c>
       <c r="P16" t="n">
-        <v>0.02969987528768473</v>
+        <v>0.1692790390533599</v>
       </c>
       <c r="Q16" t="n">
-        <v>840.2332129468787</v>
+        <v>121.27159044587</v>
       </c>
       <c r="R16" t="n">
-        <v>1343.628928617446</v>
+        <v>190.7475124633574</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>model_22_8_3</t>
+          <t>model_10_9_1</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.9993451813284396</v>
+        <v>0.9960023291556083</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8532691489467472</v>
+        <v>0.8053154670947196</v>
       </c>
       <c r="E17" t="n">
-        <v>0.999828927768586</v>
+        <v>0.9982376678205497</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9996862502127274</v>
+        <v>0.9805503162198955</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9997935104575035</v>
+        <v>0.9931333480936761</v>
       </c>
       <c r="H17" t="n">
-        <v>0.000929420049956599</v>
+        <v>0.02673244334402913</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2082631434304234</v>
+        <v>1.301856367977457</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0001447513144222854</v>
+        <v>0.0078337186681067</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0005206514013989497</v>
+        <v>0.03523159578602525</v>
       </c>
       <c r="L17" t="n">
-        <v>0.000332701133267021</v>
+        <v>0.0215326986248529</v>
       </c>
       <c r="M17" t="n">
-        <v>0.09024376705575979</v>
+        <v>0.3511748298930281</v>
       </c>
       <c r="N17" t="n">
-        <v>0.03048639122553863</v>
+        <v>0.163500591265075</v>
       </c>
       <c r="O17" t="n">
-        <v>1.000040400123695</v>
+        <v>1.003837764010616</v>
       </c>
       <c r="P17" t="n">
-        <v>0.03178426001553967</v>
+        <v>0.170461149928112</v>
       </c>
       <c r="Q17" t="n">
-        <v>839.9618995370698</v>
+        <v>105.2437546894049</v>
       </c>
       <c r="R17" t="n">
-        <v>1343.357615207637</v>
+        <v>164.9686701079467</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[12], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>model_10_9_0</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.9958891950700614</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.8046912684832226</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.9986781940409052</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.9842574318704432</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9945162855246927</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.02748897149501585</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.306030386966707</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.005875541590919013</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.02851644290185618</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.01719603276129247</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.3613699187617583</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.1657979839896006</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1.003946372732741</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.1728563474171791</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>105.1879407825823</v>
+      </c>
+      <c r="R18" t="n">
+        <v>164.9128562011241</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Hidden Size=[12], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>model_18_8_1</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9958127552793615</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.8055360048060453</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.9810097030371305</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9982512686011821</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9971359633455923</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.02800012472739863</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.300381631286339</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.01927185947342477</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.02507230761992927</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.02217209831349139</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.4423917473314977</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.1673323780007881</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1.003045268887737</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.1744560637580564</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>121.1510926285338</v>
+      </c>
+      <c r="R19" t="n">
+        <v>190.6270146460212</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>model_2_9_4</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9958065796358708</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.8044043953249312</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.9954993623091468</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.996022763627216</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9959753638190193</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.02804142128385683</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1.307948709097131</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.008590033023727631</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.04086872853353749</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.02472938077863256</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.3430050910572747</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.1674557293252662</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1.005920122867006</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.17458466640379</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>89.14814506074724</v>
+      </c>
+      <c r="R20" t="n">
+        <v>139.1220538803435</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>model_2_9_3</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.9958061018896511</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.8034127756703635</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.996106344332382</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.9972382693065854</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.9970860010570192</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0280446159750281</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1.314579674293213</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.007431531499600079</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.02837860549708563</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.01790506923086524</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.3475322915822573</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.1674652679663103</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1.005920797332257</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.174594611124531</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>89.14791721857254</v>
+      </c>
+      <c r="R21" t="n">
+        <v>139.1218260381688</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>model_2_9_5</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.9957397810515313</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.8052565685403845</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.9948362236312858</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.994674287068268</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.994744818791867</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.02848810372491505</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1.302250222881498</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.009855716585351327</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.05472521511266202</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.03229046584900667</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.338245973275162</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.1687841927578381</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1.006014426750779</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.1759696852749849</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>89.11653738401907</v>
+      </c>
+      <c r="R22" t="n">
+        <v>139.0904462036153</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>model_2_9_2</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.9957248084739243</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.8022645395788868</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.9966472255173294</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.9982815875359623</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.9980423948066279</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.02858822542031523</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1.32225793432406</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.006399191738047087</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.01765782214554312</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.0120285069417951</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.3518099660960431</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.1690805293944729</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1.006035564507401</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.1762786375757427</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>89.10952068903568</v>
+      </c>
+      <c r="R23" t="n">
+        <v>139.0834295086319</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>model_2_9_6</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.9956176606575765</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.8059850565282004</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.9941257035948021</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.9932271162342112</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.9934243899723775</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.02930472336160286</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1.297378820352594</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.01121183342848654</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.0695958505024613</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.04040384196547392</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.333292845323751</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.1711862242167952</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1.006186832012833</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.1784739761860403</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>89.06001313814181</v>
+      </c>
+      <c r="R24" t="n">
+        <v>139.033921957738</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>model_40_9_1</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.9956085905416258</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.8438718308333588</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9964641516573352</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.9845542588254076</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.9874293927947549</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0293653752687301</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1.044029786121445</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.003951968755708683</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.05500594487233312</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.02947895681402091</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.7831409986995704</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.1713632844827914</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1.00068884854249</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.1786585742741253</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>361.0558780212663</v>
+      </c>
+      <c r="R25" t="n">
+        <v>576.7968990229377</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Hidden Size=[44], regularizer=0.05, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>model_2_9_1</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.9955474638646181</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.8009411557684265</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9971103342780127</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.9991085756326383</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.9988058212569001</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.02977412963934262</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1.33110740795823</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.005515290428699157</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.009159973675988567</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.007337632403997577</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.3557988740998631</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.1725518172588821</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1.006285933367598</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.1798977053510961</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>89.0282307908487</v>
+      </c>
+      <c r="R26" t="n">
+        <v>139.0021396104449</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>model_18_8_0</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.9955075042934787</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.8051055264788338</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.9828196845164613</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.9982193805075915</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.997225072232979</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.03004133947554877</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1.303260241842572</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.0174350420298974</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.02552950081292332</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.02148225692870955</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.4511662891237886</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.1733243764608682</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1.003267269604743</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.1807031539977289</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>121.0103617266966</v>
+      </c>
+      <c r="R27" t="n">
+        <v>190.486283744184</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>Hidden Size=[14], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>model_2_9_7</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.9954507406233728</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.8066043673545532</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.9933751881187419</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.9917112302828939</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.9920402920678599</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.03042091839891943</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1.293237486005109</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.01264428659779579</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.08517257907110497</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.04890843283445038</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.3281850877725414</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.1744159350487203</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1.006422483825827</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.1818411824945036</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>88.9852496039564</v>
+      </c>
+      <c r="R28" t="n">
+        <v>138.9591584235527</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>model_2_9_0</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.9952571976650141</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.7994228321783072</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.9974821165112592</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.9996702392820124</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.9993332081304538</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.03171514105264734</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1.341260444796594</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.004805697281996149</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.003388509005067461</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.00409710326613607</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.3594793441817067</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.178087453383576</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1.006695720943509</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.1856690049659648</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>88.90192215280068</v>
+      </c>
+      <c r="R29" t="n">
+        <v>138.8758309723969</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>model_2_9_8</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.9952480728936394</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.807127557777341</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.9925915363882127</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.9901518474742772</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.9906146771924198</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.03177615844084587</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1.289738909238856</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.01413998447590489</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.1011962665545339</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.05766812477009566</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.3229608520924732</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.1782586840545107</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1.006708602973686</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.1858475252810576</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>88.89807800990422</v>
+      </c>
+      <c r="R30" t="n">
+        <v>138.8719868295005</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>Hidden Size=[10], regularizer=0.01, learning_rate=0.05</t>
         </is>
       </c>
     </row>

</xml_diff>